<commit_message>
Modified the data set creation function
</commit_message>
<xml_diff>
--- a/ticker_stocks.xlsx
+++ b/ticker_stocks.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://devinci-my.sharepoint.com/personal/thibault_le_squerent_edu_devinci_fr/Documents/Documents/éducation/ESILV/2020-2021/S7/Pi2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://devinci-my.sharepoint.com/personal/thibault_le_squerent_edu_devinci_fr/Documents/Documents/éducation/ESILV/2020-2021/S8/pi2/diffusion_indexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32B88D9B-5997-4A55-84D1-2A975D5F3CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{32B88D9B-5997-4A55-84D1-2A975D5F3CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3D8F661-36CD-4202-B3C9-90C1B45424C3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5F92E747-9B98-40F7-85C6-938196B1E081}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{5F92E747-9B98-40F7-85C6-938196B1E081}"/>
   </bookViews>
   <sheets>
     <sheet name="CAC40" sheetId="1" r:id="rId1"/>
-    <sheet name="CACNEXT20" sheetId="2" r:id="rId2"/>
-    <sheet name="S&amp;P500" sheetId="3" r:id="rId3"/>
+    <sheet name="CAC40V2" sheetId="4" r:id="rId2"/>
+    <sheet name="CACNEXT20" sheetId="2" r:id="rId3"/>
+    <sheet name="S&amp;P500" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="1167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="1172">
   <si>
     <t>Accor</t>
   </si>
@@ -3536,13 +3537,28 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>ALO.PA</t>
+  </si>
+  <si>
+    <t>EssilorLuxottica</t>
+  </si>
+  <si>
+    <t>Stellantis</t>
+  </si>
+  <si>
+    <t>STLA.PA</t>
+  </si>
+  <si>
+    <t>TEP.PA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3587,8 +3603,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3598,6 +3621,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAECF0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3641,7 +3670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3658,6 +3687,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3977,7 +4012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D220E2-844E-40A3-A141-525C4E24FA63}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -4496,6 +4531,514 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FB1B0C-2218-47D4-8963-D283DE8DCBD1}">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" tooltip="Air Liquide" display="https://en.wikipedia.org/wiki/Air_Liquide" xr:uid="{0AAABD0B-9747-4EA8-9EFE-6C36418B8426}"/>
+    <hyperlink ref="A3" r:id="rId2" tooltip="Airbus" display="https://en.wikipedia.org/wiki/Airbus" xr:uid="{C2FBC9A0-F877-4109-BD90-3EFB74E49B72}"/>
+    <hyperlink ref="A4" r:id="rId3" tooltip="Alstom" display="https://en.wikipedia.org/wiki/Alstom" xr:uid="{96F76F08-F849-4312-9620-4FB4C455ACC2}"/>
+    <hyperlink ref="A5" r:id="rId4" tooltip="ArcelorMittal" display="https://en.wikipedia.org/wiki/ArcelorMittal" xr:uid="{F1218BA5-B816-41A3-A177-4DD0B02CC2FA}"/>
+    <hyperlink ref="A6" r:id="rId5" tooltip="Atos" display="https://en.wikipedia.org/wiki/Atos" xr:uid="{3F43C507-AD6A-4AE9-8AD6-8638ECCBAF20}"/>
+    <hyperlink ref="A7" r:id="rId6" tooltip="AXA" display="https://en.wikipedia.org/wiki/AXA" xr:uid="{A890D9D7-C6ED-46FC-A8A1-816350939298}"/>
+    <hyperlink ref="A8" r:id="rId7" tooltip="BNP Paribas" display="https://en.wikipedia.org/wiki/BNP_Paribas" xr:uid="{0312D99E-BD1E-4921-864B-4AD7A98D9D5D}"/>
+    <hyperlink ref="A9" r:id="rId8" tooltip="Bouygues" display="https://en.wikipedia.org/wiki/Bouygues" xr:uid="{29045FD2-1A21-47AB-B66E-1110B0AE0F9D}"/>
+    <hyperlink ref="A10" r:id="rId9" tooltip="Capgemini" display="https://en.wikipedia.org/wiki/Capgemini" xr:uid="{1B8C6D9E-3FEC-442C-991D-6D3F6B3576D7}"/>
+    <hyperlink ref="A11" r:id="rId10" tooltip="Carrefour" display="https://en.wikipedia.org/wiki/Carrefour" xr:uid="{E63FDB10-5DBA-498B-9981-4E40ACA822B2}"/>
+    <hyperlink ref="A12" r:id="rId11" tooltip="Crédit Agricole" display="https://en.wikipedia.org/wiki/Cr%C3%A9dit_Agricole" xr:uid="{399EE549-B8CA-4C18-8BAC-3B338208D6E4}"/>
+    <hyperlink ref="A13" r:id="rId12" tooltip="Danone" display="https://en.wikipedia.org/wiki/Danone" xr:uid="{42F10C61-DAA7-4645-B7FC-C6309761D32E}"/>
+    <hyperlink ref="A14" r:id="rId13" tooltip="Dassault Systèmes" display="https://en.wikipedia.org/wiki/Dassault_Syst%C3%A8mes" xr:uid="{A910EF32-E71E-4FD8-BE05-5F7F5E886FC1}"/>
+    <hyperlink ref="A15" r:id="rId14" tooltip="Engie" display="https://en.wikipedia.org/wiki/Engie" xr:uid="{AFF084CB-68D7-4C09-A07F-1629AB0581A8}"/>
+    <hyperlink ref="A16" r:id="rId15" tooltip="EssilorLuxottica" display="https://en.wikipedia.org/wiki/EssilorLuxottica" xr:uid="{283705B0-0E90-4E60-A049-60FC484B80F7}"/>
+    <hyperlink ref="A17" r:id="rId16" tooltip="Hermès" display="https://en.wikipedia.org/wiki/Herm%C3%A8s" xr:uid="{CC31A9E4-8A7B-49C8-9FA2-371F49E7F2E4}"/>
+    <hyperlink ref="A18" r:id="rId17" tooltip="Kering" display="https://en.wikipedia.org/wiki/Kering" xr:uid="{9E0E237F-C0D1-4FF2-99EF-B9C5D41F8FE0}"/>
+    <hyperlink ref="A19" r:id="rId18" tooltip="L'Oréal" display="https://en.wikipedia.org/wiki/L%27Or%C3%A9al" xr:uid="{4B1C71F4-1ACA-4165-A8D7-C289D317100C}"/>
+    <hyperlink ref="A20" r:id="rId19" tooltip="Legrand (company)" display="https://en.wikipedia.org/wiki/Legrand_(company)" xr:uid="{0E0E522C-3EB3-4E70-A986-FDF307B95C78}"/>
+    <hyperlink ref="A21" r:id="rId20" tooltip="LVMH" display="https://en.wikipedia.org/wiki/LVMH" xr:uid="{4B42C690-2B25-4ACB-8968-04A864C98265}"/>
+    <hyperlink ref="A22" r:id="rId21" tooltip="Michelin" display="https://en.wikipedia.org/wiki/Michelin" xr:uid="{FC09C264-6C7E-492A-9DA3-DF1206D5B84B}"/>
+    <hyperlink ref="A23" r:id="rId22" tooltip="Orange S.A." display="https://en.wikipedia.org/wiki/Orange_S.A." xr:uid="{C71D1FBB-77BF-488C-9B3D-2570FA547AD6}"/>
+    <hyperlink ref="A24" r:id="rId23" tooltip="Pernod Ricard" display="https://en.wikipedia.org/wiki/Pernod_Ricard" xr:uid="{6D23718A-F595-48EB-BF91-AACF3978CEC6}"/>
+    <hyperlink ref="A25" r:id="rId24" tooltip="Publicis" display="https://en.wikipedia.org/wiki/Publicis" xr:uid="{919552BC-A678-485D-B096-CD146A678BBF}"/>
+    <hyperlink ref="A26" r:id="rId25" tooltip="Renault" display="https://en.wikipedia.org/wiki/Renault" xr:uid="{06913AF2-0EDE-4698-93D0-9F2A279464D1}"/>
+    <hyperlink ref="A27" r:id="rId26" tooltip="Safran" display="https://en.wikipedia.org/wiki/Safran" xr:uid="{32E0062B-A783-4D07-926E-38736253357F}"/>
+    <hyperlink ref="A28" r:id="rId27" tooltip="Saint-Gobain" display="https://en.wikipedia.org/wiki/Saint-Gobain" xr:uid="{387582D3-DBE0-4042-B6C0-87CCF0A03247}"/>
+    <hyperlink ref="A29" r:id="rId28" tooltip="Sanofi" display="https://en.wikipedia.org/wiki/Sanofi" xr:uid="{F989D6B6-A845-4321-937A-CA1B0C312F95}"/>
+    <hyperlink ref="A30" r:id="rId29" tooltip="Schneider Electric" display="https://en.wikipedia.org/wiki/Schneider_Electric" xr:uid="{5D442E6A-8CEE-49FE-8120-5656C1123E4C}"/>
+    <hyperlink ref="A31" r:id="rId30" tooltip="Société Générale" display="https://en.wikipedia.org/wiki/Soci%C3%A9t%C3%A9_G%C3%A9n%C3%A9rale" xr:uid="{9EECB4D0-45C4-45DC-92EB-2E0A31370EA3}"/>
+    <hyperlink ref="A32" r:id="rId31" tooltip="Stellantis" display="https://en.wikipedia.org/wiki/Stellantis" xr:uid="{EA4C0E58-D873-40C8-AADF-AD73EB128A41}"/>
+    <hyperlink ref="A33" r:id="rId32" tooltip="STMicroelectronics" display="https://en.wikipedia.org/wiki/STMicroelectronics" xr:uid="{9BCC900B-3CA3-4586-AEF6-B470F0A33BBA}"/>
+    <hyperlink ref="A34" r:id="rId33" tooltip="Teleperformance" display="https://en.wikipedia.org/wiki/Teleperformance" xr:uid="{FC556311-D656-468E-9DAD-A42FB3B695DB}"/>
+    <hyperlink ref="A35" r:id="rId34" tooltip="Thales Group" display="https://en.wikipedia.org/wiki/Thales_Group" xr:uid="{9C9CC646-701B-45B8-BA9C-7A821A727AD6}"/>
+    <hyperlink ref="A36" r:id="rId35" tooltip="Total S.A." display="https://en.wikipedia.org/wiki/Total_S.A." xr:uid="{7FFB716D-7872-48D2-85F0-A2076EA2A68E}"/>
+    <hyperlink ref="A37" r:id="rId36" tooltip="Unibail-Rodamco-Westfield" display="https://en.wikipedia.org/wiki/Unibail-Rodamco-Westfield" xr:uid="{97881134-100A-4AC0-AFCB-B2D6664496ED}"/>
+    <hyperlink ref="A38" r:id="rId37" tooltip="Veolia" display="https://en.wikipedia.org/wiki/Veolia" xr:uid="{7FF735BF-4404-4E5B-804E-EA0F8D501DF8}"/>
+    <hyperlink ref="A39" r:id="rId38" tooltip="Vinci (construction)" display="https://en.wikipedia.org/wiki/Vinci_(construction)" xr:uid="{CCAD435A-EC4C-44D4-80A2-AC407E9AF431}"/>
+    <hyperlink ref="A40" r:id="rId39" tooltip="Vivendi" display="https://en.wikipedia.org/wiki/Vivendi" xr:uid="{CBAA8B69-4DD5-4F1E-9B5A-A282A04626E8}"/>
+    <hyperlink ref="A41" r:id="rId40" tooltip="Worldline (company)" display="https://en.wikipedia.org/wiki/Worldline_(company)" xr:uid="{FFEDD628-E5EB-41F0-9AEB-BA748140BEC1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0E7156-20AA-41B4-9100-B1C3CD398CB0}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -4766,7 +5309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88D395A-9C98-46F4-88EE-B149DF1BCF2C}">
   <dimension ref="A1:C506"/>
   <sheetViews>
@@ -11363,21 +11906,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D5E3968327F484AA995A591EA850603" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="65d7e21495f06ba85f1248dd803050d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df1ebd21-298f-447d-a59d-e415769f81be" xmlns:ns4="f6f8d4a8-2cf1-48b7-9d05-4933d6248464" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd7c13181cc0c0d69822fc73e6e0f669" ns3:_="" ns4:_="">
     <xsd:import namespace="df1ebd21-298f-447d-a59d-e415769f81be"/>
@@ -11600,32 +12128,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE21770-1828-4440-AB98-7A96F9F85932}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f6f8d4a8-2cf1-48b7-9d05-4933d6248464"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="df1ebd21-298f-447d-a59d-e415769f81be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67D349C4-E136-4E3F-AA6A-FC099B1D9DED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65F44767-1C6F-4F76-BDBC-7A10A6CA01B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11642,4 +12160,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67D349C4-E136-4E3F-AA6A-FC099B1D9DED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE21770-1828-4440-AB98-7A96F9F85932}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6f8d4a8-2cf1-48b7-9d05-4933d6248464"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="df1ebd21-298f-447d-a59d-e415769f81be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>